<commit_message>
Made runmode of ordering suite to no
</commit_message>
<xml_diff>
--- a/webdriver_rediff/Suite.xlsx
+++ b/webdriver_rediff/Suite.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="13050" windowHeight="5025"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -401,7 +401,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -431,7 +431,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>